<commit_message>
Create new graphics and add to pptx and some updates to pptx
</commit_message>
<xml_diff>
--- a/docs/export_python_heuristics.xlsx
+++ b/docs/export_python_heuristics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Level 1</t>
   </si>
@@ -76,67 +76,7 @@
     <t>Level 20</t>
   </si>
   <si>
-    <t>heuristic1</t>
-  </si>
-  <si>
-    <t>0.001041</t>
-  </si>
-  <si>
-    <t>0.000143</t>
-  </si>
-  <si>
-    <t>0.0</t>
-  </si>
-  <si>
-    <t>0.007259</t>
-  </si>
-  <si>
-    <t>0.046101</t>
-  </si>
-  <si>
-    <t>0.008355</t>
-  </si>
-  <si>
-    <t>0.010536</t>
-  </si>
-  <si>
-    <t>0.02013</t>
-  </si>
-  <si>
-    <t>0.045898</t>
-  </si>
-  <si>
-    <t>0.18444</t>
-  </si>
-  <si>
-    <t>0.840127</t>
-  </si>
-  <si>
-    <t>0.014396</t>
-  </si>
-  <si>
-    <t>0.017134</t>
-  </si>
-  <si>
-    <t>0.001984</t>
-  </si>
-  <si>
-    <t>0.008058</t>
-  </si>
-  <si>
-    <t>0.028975</t>
-  </si>
-  <si>
-    <t>0.043642</t>
-  </si>
-  <si>
-    <t>0.057407</t>
-  </si>
-  <si>
-    <t>0.051588</t>
-  </si>
-  <si>
-    <t>0.067446</t>
+    <t>heuristic3</t>
   </si>
 </sst>
 </file>
@@ -566,65 +506,65 @@
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" t="s">
-        <v>34</v>
-      </c>
-      <c r="P2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2" t="s">
-        <v>38</v>
-      </c>
-      <c r="T2" t="s">
-        <v>39</v>
-      </c>
-      <c r="U2" t="s">
-        <v>40</v>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <v>8</v>
+      </c>
+      <c r="I2">
+        <v>9</v>
+      </c>
+      <c r="J2">
+        <v>8</v>
+      </c>
+      <c r="K2">
+        <v>9</v>
+      </c>
+      <c r="L2">
+        <v>11</v>
+      </c>
+      <c r="M2">
+        <v>11</v>
+      </c>
+      <c r="N2">
+        <v>11</v>
+      </c>
+      <c r="O2">
+        <v>11</v>
+      </c>
+      <c r="P2">
+        <v>11</v>
+      </c>
+      <c r="Q2">
+        <v>15</v>
+      </c>
+      <c r="R2">
+        <v>15</v>
+      </c>
+      <c r="S2">
+        <v>13</v>
+      </c>
+      <c r="T2">
+        <v>14</v>
+      </c>
+      <c r="U2">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>